<commit_message>
CT graphed profiles 1/15 script and output
</commit_message>
<xml_diff>
--- a/Data/Cond_temp/Cond_temp_logger_CalLaunch.xlsx
+++ b/Data/Cond_temp/Cond_temp_logger_CalLaunch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellebarnas/Documents/R Sessions/MooreaSGD_site-selection/Data/Cond_temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29A6A4E-2664-0D4E-AC79-43B079445FA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2979304-4267-DE49-85F2-139C32FD6A4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="11200" windowHeight="16800" xr2:uid="{94F320B9-BB3C-AE4D-AD29-F5BDA5DD55E7}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="11200" windowHeight="16800" xr2:uid="{94F320B9-BB3C-AE4D-AD29-F5BDA5DD55E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>post-calibration not stable</t>
+  </si>
+  <si>
+    <t>kept in calibration solution all day</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B947B0D1-8217-DA45-954E-4BB49A07BEF7}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,7 +970,7 @@
         <v>0.36680555555555555</v>
       </c>
       <c r="E20" s="6">
-        <v>0.41287037037037039</v>
+        <v>0.41530092592592593</v>
       </c>
       <c r="F20" s="6">
         <v>0.57814814814814819</v>
@@ -999,7 +1002,7 @@
         <v>0.37074074074074076</v>
       </c>
       <c r="E21" s="6">
-        <v>0.41287037037037039</v>
+        <v>0.41530092592592593</v>
       </c>
       <c r="F21" s="6">
         <v>0.57814814814814819</v>
@@ -1076,6 +1079,32 @@
       </c>
       <c r="J23" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>44211</v>
+      </c>
+      <c r="B24">
+        <v>319</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.36440972222222223</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.36660879629629628</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.3669560185185185</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.61880787037037044</v>
+      </c>
+      <c r="I24" s="3">
+        <v>50000</v>
+      </c>
+      <c r="J24" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calibrated CT files 1/16
</commit_message>
<xml_diff>
--- a/Data/Cond_temp/Cond_temp_logger_CalLaunch.xlsx
+++ b/Data/Cond_temp/Cond_temp_logger_CalLaunch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellebarnas/Documents/R Sessions/MooreaSGD_site-selection/Data/Cond_temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2979304-4267-DE49-85F2-139C32FD6A4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29692182-0A0A-A943-83B5-9D2CB84BF740}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="11200" windowHeight="16800" xr2:uid="{94F320B9-BB3C-AE4D-AD29-F5BDA5DD55E7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>kept in calibration solution all day</t>
+  </si>
+  <si>
+    <t>pre-calibration not stable. Post-calibration took 10 minutes to stabilize</t>
   </si>
 </sst>
 </file>
@@ -447,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B947B0D1-8217-DA45-954E-4BB49A07BEF7}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,11 +1103,136 @@
       <c r="F24" s="6">
         <v>0.61880787037037044</v>
       </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
       <c r="I24" s="3">
         <v>50000</v>
       </c>
       <c r="J24" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>44212</v>
+      </c>
+      <c r="B25">
+        <v>316</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.34699074074074071</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.49907407407407406</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.54664351851851845</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.55532407407407403</v>
+      </c>
+      <c r="I25" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>44212</v>
+      </c>
+      <c r="B26">
+        <v>316</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.49907407407407406</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.57777777777777783</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1415</v>
+      </c>
+      <c r="J26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>44212</v>
+      </c>
+      <c r="B27">
+        <v>354</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.49907407407407406</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.54664351851851845</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.55532407407407403</v>
+      </c>
+      <c r="I27" s="3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44212</v>
+      </c>
+      <c r="B28">
+        <v>354</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.35046296296296298</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.35185185185185186</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.49907407407407406</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.57777777777777783</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>